<commit_message>
[FIX] Ajuste en el scrapin
</commit_message>
<xml_diff>
--- a/web-interface/resultados.xlsx
+++ b/web-interface/resultados.xlsx
@@ -442,28 +442,28 @@
     </row>
     <row r="2" xml:space="preserve">
       <c r="A2" t="str">
-        <v>Closer SaaS B2B Startup Tecnologica</v>
+        <v>Monitora en inclusión educativa (maestro sombra)</v>
       </c>
       <c r="B2" t="str">
-        <v>La empresa es confidencial o no se encuentra disponible</v>
+        <v>CC INTEGRACION LABORAL</v>
       </c>
       <c r="C2" t="str">
-        <v>Torreón,, Coah.</v>
+        <v>CDMX</v>
       </c>
       <c r="D2" t="str">
-        <v>$20,000 - $25,000 Mensual</v>
+        <v>$8,500 Mensual</v>
       </c>
       <c r="E2" t="b">
         <v>0</v>
       </c>
       <c r="F2" t="str">
-        <v>Ventas</v>
+        <v>Educación</v>
       </c>
       <c r="G2" t="str">
-        <v>Comercial</v>
+        <v>Educación especial</v>
       </c>
       <c r="H2" t="str">
-        <v>Universitario titulado</v>
+        <v>Universitario sin titulo</v>
       </c>
       <c r="I2" t="str">
         <v>Permanente</v>
@@ -472,9 +472,59 @@
         <v>Tiempo completo</v>
       </c>
       <c r="K2" t="str">
+        <v>Presencial</v>
+      </c>
+      <c r="L2" t="str" xml:space="preserve">
+        <v xml:space="preserve">REQUISITOS:
+Nivel de estudios: Licenciatura (concluida o últimos semestres) Psicología educativa, Pedagogía, Educación especial o afines
+23 a 32 años
+Sexo indistinto
+Estado civil indistinto
+EXPERIENCIA:
+Deseable con niños con autismo, trastornos del neurodesarrollo y/o alguna discapacidad
+HABILIDADES Y COMPETENCIAS:
+Proactiva, comunicación asertiva, responsable, puntual.
+Empatía y sensibilidad emocional, paciencia, tolerancia a la frustración, vocación infantil, compromiso y responsabilidad.
+HORARIO DE TRABAJO:
+De lunes a viernes
+Interesados enviar cv a la dirección de contacto.</v>
+      </c>
+    </row>
+    <row r="3" xml:space="preserve">
+      <c r="A3" t="str">
+        <v>Closer SaaS B2B Startup Tecnologica</v>
+      </c>
+      <c r="B3" t="str">
+        <v>La empresa es confidencial o no se encuentra disponible</v>
+      </c>
+      <c r="C3" t="str">
+        <v>Torreón,, Coah.</v>
+      </c>
+      <c r="D3" t="str">
+        <v>$20,000 - $25,000 Mensual</v>
+      </c>
+      <c r="E3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3" t="str">
+        <v>Ventas</v>
+      </c>
+      <c r="G3" t="str">
+        <v>Comercial</v>
+      </c>
+      <c r="H3" t="str">
+        <v>Universitario titulado</v>
+      </c>
+      <c r="I3" t="str">
+        <v>Permanente</v>
+      </c>
+      <c r="J3" t="str">
+        <v>Tiempo completo</v>
+      </c>
+      <c r="K3" t="str">
         <v>Híbrido</v>
       </c>
-      <c r="L2" t="str" xml:space="preserve">
+      <c r="L3" t="str" xml:space="preserve">
         <v xml:space="preserve">Empresa:
 SuperLeads — Plataforma SaaS que impulsa las admisiones y la matrícula de instituciones educativas en Latinoamérica mediante tecnología inteligente y procesos comerciales impecables.
 Objetivo del rol
@@ -531,66 +581,6 @@
 Founder Comercial SuperLeads</v>
       </c>
     </row>
-    <row r="3" xml:space="preserve">
-      <c r="A3" t="str">
-        <v>Psicología</v>
-      </c>
-      <c r="B3" t="str">
-        <v>Autista Feliz, Intelig...</v>
-      </c>
-      <c r="C3" t="str">
-        <v>Veracruz,, Ver.</v>
-      </c>
-      <c r="D3" t="str">
-        <v>$6,000 Mensual</v>
-      </c>
-      <c r="E3" t="b">
-        <v>0</v>
-      </c>
-      <c r="F3" t="str">
-        <v>Educación</v>
-      </c>
-      <c r="G3" t="str">
-        <v>Psicopedagogía</v>
-      </c>
-      <c r="H3" t="str">
-        <v>Universitario titulado</v>
-      </c>
-      <c r="I3" t="str">
-        <v>Permanente</v>
-      </c>
-      <c r="J3" t="str">
-        <v>Medio tiempo</v>
-      </c>
-      <c r="K3" t="str">
-        <v>Presencial</v>
-      </c>
-      <c r="L3" t="str" xml:space="preserve">
-        <v xml:space="preserve">Lic. En Psicología para Evaluación e Intervención en Autismo
-Ubicación: Veracruz, Ver.
-Modalidad: Presencial | Medio tiempo (vespertino) por honorarios.
-Descripción del puesto:
-En AFII buscamos profesionales comprometidos y empáticos para integrarse a nuestro equipo de atención terapéutica y evaluación psicológica dirigida a personas dentro del espectro autista (niños, adolescentes y adultos). El puesto implica la planeación, ejecución y seguimiento de sesiones de intervención psicológica, así como la aplicación de evaluaciones psicológicas.
-Responsabilidades:
-Brindar terapia psicológica individualizada a personas autistas.
-Aplicar evaluaciones psicológicas según el perfil y necesidades del paciente.
-Realizarobservaciones.
-Elaborar planeaciones de las sesiones y actualizar planes de trabajo.
-Trabajar en colaboración con el equipo multidisciplinario.
-Mantener una comunicación efectiva con los cuidadores principales, equipo de terapeutas y dirección.
-Requisitos:
-Licenciatura en Psicología (indispensable contar con título y cédula profesional).
-Gusto y vocación por trabajar con personas dentro del espectro autista.
-Experiencia con población infantil, adolescente y/o adulta (preferente).
-Ser una persona responsable, empática y con disposición para el aprendizaje continuo.
-Ofrecemos:
-Uniformes.
-Bonotrimestral por evaluación de desempeño.
-Honorarios con incremento en caso de contar con maestría en áreas afines (educación especial, neuropsicología, intervención en autismo, entre otras).
-Horario vespertino: lunes a viernes, entrada 2:50, salida 7:00 pm.
-¿Te interesa formar parte de nuestro equipo?</v>
-      </c>
-    </row>
     <row r="4" xml:space="preserve">
       <c r="A4" t="str">
         <v>TERAPEUTA ESPECIALIZADA EN TEA Y TDAH</v>

</xml_diff>

<commit_message>
[ADD]Se agrego la practica
</commit_message>
<xml_diff>
--- a/web-interface/resultados.xlsx
+++ b/web-interface/resultados.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -442,19 +442,19 @@
     </row>
     <row r="2" xml:space="preserve">
       <c r="A2" t="str">
-        <v>Maestra</v>
+        <v>Acompañante de menor o Maestro Sombra</v>
       </c>
       <c r="B2" t="str">
-        <v>Asociación Centro de T...</v>
+        <v>La empresa es confidencial o no se encuentra disponible</v>
       </c>
       <c r="C2" t="str">
-        <v>SLP.</v>
+        <v>Hermosillo,, Son.</v>
       </c>
       <c r="D2" t="str">
-        <v>$5,000 - $6,000 Mensual</v>
+        <v>$12,000 Mensual</v>
       </c>
       <c r="E2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2" t="str">
         <v>Educación</v>
@@ -469,12 +469,284 @@
         <v>Permanente</v>
       </c>
       <c r="J2" t="str">
+        <v>Tiempo completo</v>
+      </c>
+      <c r="K2" t="str">
+        <v>Presencial</v>
+      </c>
+      <c r="L2" t="str" xml:space="preserve">
+        <v xml:space="preserve">Vacante: Acompañante de niño (TDA o Autismo) – Maestro Sombra
+Ubicación: Zona Poniente, Hermosillo
+Horario: lunes a viernes
+Requisitos:
+Sexo indistinto
+Carrera en Pedagogía, Ciencias de la Educación o afín
+Especialidad o experiencia en Educación Especial
+Experiencia como maestro sombra o acompañante educativo
+Paciencia, empatía y habilidades de comunicación
+Responsabilidad y compromiso
+Preferente cuente con carro para su traslado
+Funciones principales:
+Brindar apoyo personalizado a un niño con TDA o Trastorno del Espectro Autista en su entorno escolar
+Favorecer la integración e inclusión en actividades académicas y sociales
+Implementar estrategias de apoyo de acuerdo con el plan educativo
+Colaborar con docentes y padres para dar seguimiento al progreso
+Ofrecemos:
+Contratación directa
+Estabilidad laboral
+Ambiente de trabajo respetuoso y colaborativo</v>
+      </c>
+    </row>
+    <row r="3" xml:space="preserve">
+      <c r="A3" t="str">
+        <v>Terapeuta</v>
+      </c>
+      <c r="B3" t="str">
+        <v>La empresa es confidencial o no se encuentra disponible</v>
+      </c>
+      <c r="C3" t="str">
+        <v>León,, Gto.</v>
+      </c>
+      <c r="D3" t="str">
+        <v>$14,000 - $16,000 Mensual</v>
+      </c>
+      <c r="E3" t="b">
+        <v>1</v>
+      </c>
+      <c r="F3" t="str">
+        <v>Sector salud</v>
+      </c>
+      <c r="G3" t="str">
+        <v>Terapeuta</v>
+      </c>
+      <c r="H3" t="str">
+        <v>Universitario titulado</v>
+      </c>
+      <c r="I3" t="str">
+        <v>Permanente</v>
+      </c>
+      <c r="J3" t="str">
+        <v>Tiempo completo</v>
+      </c>
+      <c r="K3" t="str">
+        <v>Presencial</v>
+      </c>
+      <c r="L3" t="str" xml:space="preserve">
+        <v xml:space="preserve">Requisitos del puesto
+Estudios universitarios con título en Terapia.
+Experiencia previa como Terapeuta de niños con Trastornos del espectro autista.
+Gusto por realizar manualidades.
+Habilidad para nadar.
+Licencia de manejo vigente.
+Conocimientos en técnicas de terapia y rehabilitación.
+Licencia o certificación válida en Terapia (deseable).
+Responsabilidades del puesto
+Realizar evaluaciones y diagnósticos de los pacientes.
+Diseñar planes de tratamiento personalizados.
+Realizar sesiones de terapia adaptadas a las necesidades individuales de cada paciente.
+Mantener registros precisos de la evolución de los pacientes.
+Prestaciones y beneficios adicionales
+Salario mensual competitivo de 14000 a 16000.
+Prestaciones de ley.
+Vales de despensa.
+Fondo de ahorro.
+Oportunidades de capacitación y desarrollo profesional en un ambiente de trabajo colaborativo y en constante crecimiento.</v>
+      </c>
+    </row>
+    <row r="4" xml:space="preserve">
+      <c r="A4" t="str">
+        <v>Psicología clínica</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Fundación Planeta Tea AC</v>
+      </c>
+      <c r="C4" t="str">
+        <v>San Pedro Garza García,, N.L.</v>
+      </c>
+      <c r="D4" t="str">
+        <v>$14,000 - $15,000 Mensual</v>
+      </c>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F4" t="str">
+        <v>Ciencias sociales - Humanidades</v>
+      </c>
+      <c r="G4" t="str">
+        <v>Psicología</v>
+      </c>
+      <c r="H4" t="str">
+        <v>Universitario titulado</v>
+      </c>
+      <c r="I4" t="str">
+        <v>Permanente</v>
+      </c>
+      <c r="J4" t="str">
+        <v>Tiempo completo</v>
+      </c>
+      <c r="K4" t="str">
+        <v>Presencial</v>
+      </c>
+      <c r="L4" t="str" xml:space="preserve">
+        <v xml:space="preserve">Acerca de la empresa
+Fundación Planeta Tea AC es una organización dedicada a apoyar a niños y adultos con autismo de escasos recursos y sus familias, brindando servicios de psicología clínica y terapias especializadas. Nuestra misión es mejorar la calidad de vida de las personas con autismo a través de la educación y la inclusión en la sociedad. Al unirte a nuestro equipo, tendrás la oportunidad de contribuir a una causa noble y en constante crecimiento, además de recibir apoyo y capacitación continua. Ubicación: San Pedro Garza García, Nuevo León.
+Requisitos del puesto
+Educación mínima: Universitario con título y cédula profesional en Psicología
+Experiencia y conocimiento en la aplicación de pruebas psicológicas.
+Experiencia en pacientes con autismo de mínimo 1 año y 3 años deseable.
+Responsabilidades del puesto
+Evaluación emocional y conductual
+Psicoterapia individual y familiar
+Apoyo en planes educativos individualizados.
+Manejo de citas
+Coordinación de personal
+Prestaciones y beneficios adicionales
+Prestaciones de ley
+Salario mensual de 14000 a 15000.
+Bonos incentivos
+Horario a tiempo completo: Lunes a viernes de 10am a 7pm, con 1 hora de comida y Sábados de 9am a 1:30pm horario corrido.
+Modalidad presencial.
+Oportunidades de capacitación y desarrollo profesional.
+Excelente ambiente de trabajo.</v>
+      </c>
+    </row>
+    <row r="5" xml:space="preserve">
+      <c r="A5" t="str">
+        <v>Monitora en inclusión educativa (maestro sombra)</v>
+      </c>
+      <c r="B5" t="str">
+        <v>CC INTEGRACION LABORAL</v>
+      </c>
+      <c r="C5" t="str">
+        <v>CDMX</v>
+      </c>
+      <c r="D5" t="str">
+        <v>$8,500 Mensual</v>
+      </c>
+      <c r="E5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F5" t="str">
+        <v>Educación</v>
+      </c>
+      <c r="G5" t="str">
+        <v>Educación especial</v>
+      </c>
+      <c r="H5" t="str">
+        <v>Universitario sin titulo</v>
+      </c>
+      <c r="I5" t="str">
+        <v>Permanente</v>
+      </c>
+      <c r="J5" t="str">
+        <v>Tiempo completo</v>
+      </c>
+      <c r="K5" t="str">
+        <v>Presencial</v>
+      </c>
+      <c r="L5" t="str" xml:space="preserve">
+        <v xml:space="preserve">REQUISITOS:
+Nivel de estudios: Licenciatura (concluida o últimos semestres) Psicología educativa, Pedagogía, Educación especial o afines
+23 a 32 años
+Sexo indistinto
+Estado civil indistinto
+EXPERIENCIA:
+Deseable con niños con autismo, trastornos del neurodesarrollo y/o alguna discapacidad
+HABILIDADES Y COMPETENCIAS:
+Proactiva, comunicación asertiva, responsable, puntual.
+Empatía y sensibilidad emocional, paciencia, tolerancia a la frustración, vocación infantil, compromiso y responsabilidad.
+HORARIO DE TRABAJO:
+De lunes a viernes
+Interesados enviar cv a la dirección de contacto.</v>
+      </c>
+    </row>
+    <row r="6" xml:space="preserve">
+      <c r="A6" t="str">
+        <v>Psicóloga</v>
+      </c>
+      <c r="B6" t="str">
+        <v>Neuro Activa</v>
+      </c>
+      <c r="C6" t="str">
+        <v>CDMX</v>
+      </c>
+      <c r="D6" t="str">
+        <v>$8,364 - $8,500 Mensual</v>
+      </c>
+      <c r="E6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F6" t="str">
+        <v>Educación</v>
+      </c>
+      <c r="G6" t="str">
+        <v>Psicopedagogía</v>
+      </c>
+      <c r="H6" t="str">
+        <v>Universitario titulado</v>
+      </c>
+      <c r="I6" t="str">
+        <v>Permanente</v>
+      </c>
+      <c r="J6" t="str">
+        <v>Tiempo completo</v>
+      </c>
+      <c r="K6" t="str">
+        <v>Híbrido</v>
+      </c>
+      <c r="L6" t="str" xml:space="preserve">
+        <v xml:space="preserve">Acerca de la empresa
+Neuro Activa es una empresa líder en el campo de la educación y la psicopedagogía, comprometida con el desarrollo integral de cada individuo. Trabajar con nosotros significa formar parte de un equipo dedicado a brindar soluciones innovadoras y personalizadas a las necesidades educativas especiales. - Ubicación: Ciudad de México.
+Requisitos del puesto
+Licenciatura en Psicología, Educación Especial, Pedagogía, Psicopedagogía o afines.
+Diplomado o curso en intervención educativa, inclusión escolar o TEA/TDAH. (Deseable)
+Experiencia mínima de 6 meses con niños con necesidades educativas especiales (NEE), Trastorno del Espectro Autista (TEA), TDAH u otras condiciones del neurodesarrollo.
+Conocimientos básicos de adaptaciones curriculares y manejo de conductas.
+Habilidades en regulación emocional, contención y acompañamiento respetuoso.
+Capacidad para implementar estrategias sensoriales, estructuración del entorno y apoyos visuales.
+Buen manejo de la comunicación con familia y equipo docente.
+Responsabilidades del puesto
+Brindar intervención educativa y apoyo a niños con necesidades educativas especiales.
+Implementar estrategias de inclusión escolar y adaptaciones curriculares.
+Colaborar con el equipo docente y familia en el desarrollo del plan de intervención individualizado.
+Únete a nuestro equipo en Neuro Activa y sé parte de un proyecto que transforma vidas a través de la educación inclusiva. ¡Aplica ahora y haz la diferencia!</v>
+      </c>
+    </row>
+    <row r="7" xml:space="preserve">
+      <c r="A7" t="str">
+        <v>Maestra</v>
+      </c>
+      <c r="B7" t="str">
+        <v>Asociación Centro de T...</v>
+      </c>
+      <c r="C7" t="str">
+        <v>SLP.</v>
+      </c>
+      <c r="D7" t="str">
+        <v>$5,000 - $6,000 Mensual</v>
+      </c>
+      <c r="E7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F7" t="str">
+        <v>Educación</v>
+      </c>
+      <c r="G7" t="str">
+        <v>Educación especial</v>
+      </c>
+      <c r="H7" t="str">
+        <v>Universitario titulado</v>
+      </c>
+      <c r="I7" t="str">
+        <v>Permanente</v>
+      </c>
+      <c r="J7" t="str">
         <v>Medio tiempo</v>
       </c>
-      <c r="K2" t="str">
+      <c r="K7" t="str">
         <v>Híbrido</v>
       </c>
-      <c r="L2" t="str" xml:space="preserve">
+      <c r="L7" t="str" xml:space="preserve">
         <v xml:space="preserve">Acerca de la empresa
 **** Asociación Centro de Terapia Infantil y de Educación Especial es una organización comprometida con el bienestar y desarrollo de niños, niñas y jóvenes con autismo, síndrome de Down y/o discapacidad intelectual. Nuestra misión es brindar un ambiente inclusivo y terapéutico para promover su crecimiento y aprendizaje. - **Ubicación:** San Luis Potosí.
 Requisitos del puesto
@@ -494,215 +766,9 @@
 Ambiente de trabajo colaborativo y respetuoso.</v>
       </c>
     </row>
-    <row r="3" xml:space="preserve">
-      <c r="A3" t="str">
-        <v>Monitora en inclusión educativa (maestro sombra)</v>
-      </c>
-      <c r="B3" t="str">
-        <v>CC INTEGRACION LABORAL</v>
-      </c>
-      <c r="C3" t="str">
-        <v>CDMX</v>
-      </c>
-      <c r="D3" t="str">
-        <v>$8,500 Mensual</v>
-      </c>
-      <c r="E3" t="b">
-        <v>0</v>
-      </c>
-      <c r="F3" t="str">
-        <v>Educación</v>
-      </c>
-      <c r="G3" t="str">
-        <v>Educación especial</v>
-      </c>
-      <c r="H3" t="str">
-        <v>Universitario sin titulo</v>
-      </c>
-      <c r="I3" t="str">
-        <v>Permanente</v>
-      </c>
-      <c r="J3" t="str">
-        <v>Tiempo completo</v>
-      </c>
-      <c r="K3" t="str">
-        <v>Presencial</v>
-      </c>
-      <c r="L3" t="str" xml:space="preserve">
-        <v xml:space="preserve">REQUISITOS:
-Nivel de estudios: Licenciatura (concluida o últimos semestres) Psicología educativa, Pedagogía, Educación especial o afines
-23 a 32 años
-Sexo indistinto
-Estado civil indistinto
-EXPERIENCIA:
-Deseable con niños con autismo, trastornos del neurodesarrollo y/o alguna discapacidad
-HABILIDADES Y COMPETENCIAS:
-Proactiva, comunicación asertiva, responsable, puntual.
-Empatía y sensibilidad emocional, paciencia, tolerancia a la frustración, vocación infantil, compromiso y responsabilidad.
-HORARIO DE TRABAJO:
-De lunes a viernes
-Interesados enviar cv a la dirección de contacto.</v>
-      </c>
-    </row>
-    <row r="4" xml:space="preserve">
-      <c r="A4" t="str">
-        <v>TERAPEUTA ESPECIALIZADA EN TEA Y TDAH</v>
-      </c>
-      <c r="B4" t="str">
-        <v>La empresa es confidencial o no se encuentra disponible</v>
-      </c>
-      <c r="C4" t="str">
-        <v>CDMX</v>
-      </c>
-      <c r="D4" t="str">
-        <v>$9,000 - $12,000 Mensual</v>
-      </c>
-      <c r="E4" t="b">
-        <v>1</v>
-      </c>
-      <c r="F4" t="str">
-        <v>Ciencias sociales - Humanidades</v>
-      </c>
-      <c r="G4" t="str">
-        <v>Psicología</v>
-      </c>
-      <c r="H4" t="str">
-        <v>Universitario sin titulo</v>
-      </c>
-      <c r="I4" t="str">
-        <v>Permanente</v>
-      </c>
-      <c r="J4" t="str">
-        <v>Tiempo completo</v>
-      </c>
-      <c r="K4" t="str">
-        <v>Presencial</v>
-      </c>
-      <c r="L4" t="str" xml:space="preserve">
-        <v xml:space="preserve">TERAPEUTA ESPECIALIZADA EN TEA Y TDAH
-Fundación Valentina – Benito Juárez, Ciudad de México, Anaxágoras 25, Col. Piedad Narvarte, Alcaldía Benito Juárez, CDMX.
-Horario: Lunes a viernes de 8:30 a 18:00 hrs
-Sueldo: $9,000 a $12,000 mensuales (según experiencia)
-OBJETIVO DEL PUESTO
-Brindar atención terapéutica especializada a niños, niñas y adolescentes con diagnóstico de Trastorno del Espectro Autista (TEA) y/o Trastorno por Déficit de Atención e Hiperactividad (TDAH), mediante un enfoque individualizado que favorezca su desarrollo integral, habilidades sociales, comunicación, autorregulación y autonomía.
-PERFIL REQUERIDO
-Sexo: Femenino
-Edad: 25 a 30 años
-Escolaridad: Licenciatura en Psicología (PRINCIPALEMENTE PSICOLOGIA CLINICA), Psicopedagogía, Pedagogía o Terapia Ocupacional, con especialidad o formación en educación especial, neurodiversidad o neurociencias (Indispensable contar con título y cédula profesional o en proceso).
-Formación adicional deseable: Diplomados o certificaciones en ABA, PECS, TEACCH, Denver o afines.
-Experiencia mínima: 1 año comprobable trabajando con población TEA y/o TDAH.
-Residencia: No vivir a más de una hora de distancia del centro.
-HABILIDADES CLAVES
-Saber realizar diagnósticos y valoraciones en TEA y TDAH. ?
-Diseño e implementación de planes terapéuticos individuales.
-Elaboración de bitácoras y reportes terapéuticos.
-Trabajo colaborativo y orientación a familias.
-Alta empatía, responsabilidad, comunicación y observación clínica.
-FUNCIONES PRINCIPALES
-Realización de valoraciones y diagnósticos clínico-funcionales en TEA y TDAH.
-Diseño y aplicación de intervenciones personalizadas.
-Elaboración y entrega mensual de planeaciones terapéuticas.
-Registro y envío de bitácoras mensuales.
-Aplicación de técnicas conductuales y metodologías estructuradas.
-Trabajo coordinado con equipo multidisciplinario.
-Asesoramiento continuo a padres de familia.
-SOLO POSTULARSE SI CUMPLES CON LOS REQUISITOS DEL PERFIL, SOLO PSICOLOGAS CLINICAS ESPECIALIZADAS EN TEA Y TDAH, NO LABORALES</v>
-      </c>
-    </row>
-    <row r="5" xml:space="preserve">
-      <c r="A5" t="str">
-        <v>Closer SaaS B2B Startup Tecnologica</v>
-      </c>
-      <c r="B5" t="str">
-        <v>La empresa es confidencial o no se encuentra disponible</v>
-      </c>
-      <c r="C5" t="str">
-        <v>Torreón,, Coah.</v>
-      </c>
-      <c r="D5" t="str">
-        <v>$20,000 - $25,000 Mensual</v>
-      </c>
-      <c r="E5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F5" t="str">
-        <v>Ventas</v>
-      </c>
-      <c r="G5" t="str">
-        <v>Comercial</v>
-      </c>
-      <c r="H5" t="str">
-        <v>Universitario titulado</v>
-      </c>
-      <c r="I5" t="str">
-        <v>Permanente</v>
-      </c>
-      <c r="J5" t="str">
-        <v>Tiempo completo</v>
-      </c>
-      <c r="K5" t="str">
-        <v>Híbrido</v>
-      </c>
-      <c r="L5" t="str" xml:space="preserve">
-        <v xml:space="preserve">Empresa:
-SuperLeads — Plataforma SaaS que impulsa las admisiones y la matrícula de instituciones educativas en Latinoamérica mediante tecnología inteligente y procesos comerciales impecables.
-Objetivo del rol
-Ser la primera línea de crecimiento de SuperLeads: realizar prospección outbound diaria (llamadas, correos y LinkedIn) a nuestro *Ideal Customer Profile* (ICP) para generar al menos 30 conexiones efectivas por día y agendar citas calificadas para nuestro equipo de Account Executives.
-Responsabilidades clave
-Ejecutar cadencias multicanal (teléfono, email, LinkedIn) y mantener registro de todo en SuperLeads &lt;- Usas el mejor CRM para vender el mejor CRM educativo, tu capacitación de explicación esta intimamente ligada a tu uso del CRM para vender!
-Detectar necesidades, calificar leads con criterio Bajo, Medio, Alto y concertar reuniones.
-Alcanzar meta semanal de citas asistidas y tasa de respuesta mínima del 15 %.
-Colaborar con Marketing para nutrir leads y con Closers para retroalimentación de calidad.
-Participar en role-plays, coaching, Talleres, Congresos y workshops internos para elevar tu pitch.
-Representar la cultura SuperLeads: presencia real, comunicación consciente y ritmo sostenible.
-Compensación
-Sueldo base: $12,000 MXN brutos/mes
-De $500 MXN a $5,000 MXN por cada cita calificada que se lleve a cabo.
-Ingreso estimado: $40,000 MXN/mes (base + comisiones). &lt;- Buscamos solo gente responsable
-Prestaciones de ley, laptop y línea telefónica corporativa.
-Requisitos
-5 + año en prospección o telemarketing B2B (ventas SaaS o educación, deseable).
-Dominio de llamadas en frío (que no te de miedo ni flojera), redacción de correos y social-selling en LinkedIn, que te guste escribir.
-Conocimiento básico de CRM (HubSpot o similar) y hábito de documentación rigurosa.
-Actitud hunter (eres un cazador y no paras hasta lograr la cita), resiliencia ante la objeción y enfoque a métricas diarias.
-Excelente ortografía y dicción; gusto por aprender y aportar ideas.
-Disponibilidad tiempo completo en oficina de Torreón.
-Lo que ofrecemos
-Plan de carrera claro a Closer en 12-18 meses según performance.
-Formación continua en metodologías de venta consultiva (SPIN, MEDDICC, Challenger).
-Ambiente de alto desempeño con calidez humana: celebramos logros y cuidamos el bienestar.
-Propósito de impacto: ayudar a colegios y universidades a transformar sus admisiones.
----
-¿Te apasiona la prospección, el contacto humano y el mundo EdTech?
-¡Únete a SuperLeads y conviértete en la chispa que encienda el crecimiento educativo en LATAM!
-Tipo de puesto: Tiempo completo
-Sueldo: A partir de $12,000 MXN al mes &lt;- Esto es el inicial, si no ganas 3 veces más esto al menos, te descontraríamos por que nos hacemos daño, nos gusta que las personas con nosotros gane bien y esto lo demuestra.
-Beneficios:
-Aumentos salariales ritmo Startup
-Días de paternidad superiores a los de la ley
-Laptop y celular de la empresa
-&gt;100 Ventas, Carro de la empresa
-Pago complementario:
-Bono anual &gt;52 ventas en el año
-Bono de productividad Pago por Cita asistida
-Tipo de jornada:
-55 horas semanales mínimo
-Como tu las acomodes
-Pregunta(s) de postulación: (Es importante que tengamos estas respuestas.
-Describe en 2-3 líneas tu logro laboral más sobresaliente
-Si te contratamos, ¿cómo serían tus primeros 100 días en SuperLeads?
-¿Tu puesto como impacta directamente los ingresos de la empresa, exactamente?
-Lugar de trabajo: Empleo presencial o Híbrido.
-Fecha de inicio prevista: 01/08/2025
-Solo aplica si crees que eres Player A, osea un Mini-Ceo, entrepeneur, Motivado siempre, Con deficit de atención, Autismo.
-Nos vemos pronto ó no.
-Ing. Ricardo López Reyero
-Founder Comercial SuperLeads</v>
-      </c>
-    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L7"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>